<commit_message>
Added relative FPR/FNR and fixed reference to XNN
</commit_message>
<xml_diff>
--- a/data/output/Disparity Tables for Paper.xlsx
+++ b/data/output/Disparity Tables for Paper.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Artificial Intelligence\article-information-2019\data\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3EF4BEC4-AF93-461A-95D8-FB1C57E8DDF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D4DF30-60FF-4E5B-AF8B-EF70E3FA7C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1845" windowWidth="28800" windowHeight="15435"/>
+    <workbookView xWindow="20745" yWindow="3720" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 2 - Simulated" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,15 @@
     <sheet name="Table 6 - HMDA" sheetId="5" r:id="rId4"/>
     <sheet name="DATA" sheetId="1" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -113,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
@@ -987,11 +995,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1248,7 +1256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1256,7 +1264,7 @@
       <selection activeCell="D12" sqref="D12"/>
       <selection pane="topRight" activeCell="D12" sqref="D12"/>
       <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1460,7 +1468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1468,7 +1476,7 @@
       <selection activeCell="D12" sqref="D12"/>
       <selection pane="topRight" activeCell="D12" sqref="D12"/>
       <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1725,7 +1733,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1733,7 +1741,7 @@
       <selection activeCell="D12" sqref="D12"/>
       <selection pane="topRight" activeCell="D12" sqref="D12"/>
       <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1940,14 +1948,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>

</xml_diff>